<commit_message>
V3: better handling of electives, and some pre-reqs. Can process all BICT students.
</commit_message>
<xml_diff>
--- a/Course Progression BICT.xlsx
+++ b/Course Progression BICT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utting/usc_onedrive/OneDrive - University of the Sunshine Coast/workspace_jupyter/research/cir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964442CF-61F5-CC4E-96C8-68612917D227}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="114_{824C6520-E5D7-B942-86CF-B80AA9609D3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2E3049FB-0591-1845-B419-73E16B5C3127}"/>
   <bookViews>
-    <workbookView xWindow="-36880" yWindow="-3560" windowWidth="28460" windowHeight="18180" xr2:uid="{42803720-E939-4A64-84C4-AFDAB47A9612}"/>
+    <workbookView xWindow="-38120" yWindow="-3400" windowWidth="23660" windowHeight="18180" xr2:uid="{42803720-E939-4A64-84C4-AFDAB47A9612}"/>
   </bookViews>
   <sheets>
     <sheet name="BICT" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="95">
   <si>
     <t>Progression value</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>Elective Level 200</t>
+  </si>
+  <si>
+    <t>needs to be earlier if sem2 start</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -779,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E5F594-2D66-49DC-8222-7DDA3D39318A}">
-  <dimension ref="B1:J53"/>
+  <dimension ref="B1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -790,7 +796,7 @@
     <col min="2" max="2" width="17.5" style="6" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="41.5" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="6"/>
+    <col min="5" max="5" width="25.83203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -809,7 +815,9 @@
       <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="6">
@@ -1098,7 +1106,9 @@
       <c r="D29" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="11"/>
+      <c r="E29" s="11" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B30" s="6">
@@ -1114,7 +1124,7 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B31" s="6">
-        <v>1.131</v>
+        <v>1.133</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
@@ -1236,6 +1246,9 @@
       <c r="D41" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="E41" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="42" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="24">
@@ -1335,39 +1348,39 @@
       </c>
       <c r="E49" s="21"/>
     </row>
-    <row r="50" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="24">
-        <v>6.3319999999999999</v>
-      </c>
-      <c r="C50" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="24"/>
+    <row r="50" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="21">
+        <v>5.37</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E50" s="21"/>
     </row>
     <row r="51" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B51" s="24">
         <v>6.3319999999999999</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E51" s="24"/>
     </row>
     <row r="52" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B52" s="24">
-        <v>6.3819999999999997</v>
+        <v>6.3319999999999999</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="E52" s="24"/>
     </row>
@@ -1382,6 +1395,18 @@
         <v>87</v>
       </c>
       <c r="E53" s="24"/>
+    </row>
+    <row r="54" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="24">
+        <v>6.3819999999999997</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E54" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -2042,15 +2067,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C581CD223B8CC7429F2C04820162A271" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b3f372d8b489231ef829fb4ffe146bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5915d4c3-9fb8-4d5f-bc44-8b6704948b94" xmlns:ns4="83e39629-3244-4ebf-a277-aa7822261d47" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c02e1a779c207581108d353a3468fd4e" ns3:_="" ns4:_="">
     <xsd:import namespace="5915d4c3-9fb8-4d5f-bc44-8b6704948b94"/>
@@ -2259,21 +2275,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{772B05B0-3DD5-4BFB-B4E9-5EA5AEE0168F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF67D51E-13E1-481C-8529-F4CACB0EB3D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2292,19 +2309,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAD9A558-79BD-4FA9-AD18-81B496DD988B}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="83e39629-3244-4ebf-a277-aa7822261d47"/>
+    <ds:schemaRef ds:uri="5915d4c3-9fb8-4d5f-bc44-8b6704948b94"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="83e39629-3244-4ebf-a277-aa7822261d47"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5915d4c3-9fb8-4d5f-bc44-8b6704948b94"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{772B05B0-3DD5-4BFB-B4E9-5EA5AEE0168F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>